<commit_message>
done merging conversion and new
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/FEEDSTOCKS.xlsx
+++ b/cea/databases/CH/components/FEEDSTOCKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC15C70D-FFCE-9C4B-A03B-533BA3868A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A982472-3F41-B441-95FC-85BAC176F9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="500" windowWidth="46580" windowHeight="27340" tabRatio="993" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="500" windowWidth="46580" windowHeight="27340" tabRatio="993" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRID" sheetId="28" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="OIL" sheetId="30" r:id="rId6"/>
     <sheet name="NATURALGAS" sheetId="22" r:id="rId7"/>
     <sheet name="BIOGAS" sheetId="27" r:id="rId8"/>
-    <sheet name="SOLAR" sheetId="29" r:id="rId9"/>
-    <sheet name="HYDROGEN" sheetId="36" r:id="rId10"/>
+    <sheet name="HYDROGEN" sheetId="36" r:id="rId9"/>
+    <sheet name="SOLAR" sheetId="29" r:id="rId10"/>
     <sheet name="ENERGY_CARRIERS" sheetId="35" r:id="rId11"/>
   </sheets>
   <definedNames>
@@ -99,7 +99,7 @@
     <author>Jimeno</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{91F6A146-4E75-014C-925E-06C33CC2B2BB}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -112,12 +112,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{B71303BF-00AE-9F48-B64E-62E24C7DEA25}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{4686B76A-F401-414D-904C-E4BF85BE0E37}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -491,7 +491,7 @@
     <author>Jimeno</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{91F6A146-4E75-014C-925E-06C33CC2B2BB}">
       <text>
         <r>
           <rPr>
@@ -504,12 +504,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{B71303BF-00AE-9F48-B64E-62E24C7DEA25}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -517,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{4686B76A-F401-414D-904C-E4BF85BE0E37}">
       <text>
         <r>
           <rPr>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="149">
   <si>
     <t>reference</t>
   </si>
@@ -1133,10 +1133,13 @@
     <t>Infrared light</t>
   </si>
   <si>
-    <t>Shall we update the ghg and cost based on the SOLAR Tab?</t>
-  </si>
-  <si>
     <t>This should be linked to GRID Tab</t>
+  </si>
+  <si>
+    <t>to be deleted</t>
+  </si>
+  <si>
+    <t>Shall we update the SOLAR Tab and change everything to zero?</t>
   </si>
 </sst>
 </file>
@@ -2340,17 +2343,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230A53B8-EB6F-684C-8324-7AC0C54FE34E}">
-  <dimension ref="A1:N64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P73" sqref="I48:P73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -2375,16 +2381,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C2" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D2" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2392,16 +2398,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C3" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D3" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2409,16 +2415,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C4" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D4" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2426,16 +2432,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C5" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D5" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>137</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2443,16 +2449,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C6" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D6" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2460,16 +2466,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C7" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D7" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2477,16 +2483,16 @@
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C8" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.6</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2494,16 +2500,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C9" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2511,16 +2517,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C10" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D10" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>137</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2528,16 +2534,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C11" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D11" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2545,16 +2551,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C12" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D12" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2562,16 +2568,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C13" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.6</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>137</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2579,16 +2585,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C14" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D14" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.6</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>137</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2596,16 +2602,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C15" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.6</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2613,16 +2619,16 @@
         <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C16" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D16" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2630,16 +2636,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C17" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D17" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.6</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2647,16 +2653,16 @@
         <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C18" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D18" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2664,16 +2670,16 @@
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C19" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D19" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>137</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2681,16 +2687,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C20" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D20" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2698,16 +2704,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C21" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D21" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.6</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2715,16 +2721,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C22" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D22" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>137</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2732,16 +2738,16 @@
         <v>25</v>
       </c>
       <c r="B23" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C23" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D23" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.6</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2749,16 +2755,16 @@
         <v>26</v>
       </c>
       <c r="B24" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C24" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D24" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.6</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2766,21 +2772,17 @@
         <v>27</v>
       </c>
       <c r="B25" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C25" s="16">
-        <v>0.2261</v>
-      </c>
-      <c r="D25" s="16">
-        <v>0.2261</v>
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.6</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="64" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2790,10 +2792,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468519ED-3798-6A47-8D33-1999B16E1C77}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3196,7 +3198,7 @@
         <v>104</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -3551,7 +3553,7 @@
         <v>142</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -3616,6 +3618,11 @@
       </c>
       <c r="J26" s="15" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="21" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -7177,20 +7184,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230A53B8-EB6F-684C-8324-7AC0C54FE34E}">
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E25"/>
+      <selection activeCell="P73" sqref="I48:P73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -7215,16 +7219,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -7232,16 +7236,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7249,16 +7253,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -7266,16 +7270,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -7283,16 +7287,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -7300,16 +7304,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -7317,16 +7321,16 @@
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -7334,16 +7338,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -7351,16 +7355,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -7368,16 +7372,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -7385,16 +7389,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -7402,16 +7406,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -7419,16 +7423,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>39</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -7436,16 +7440,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -7453,16 +7457,16 @@
         <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -7470,16 +7474,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -7487,16 +7491,16 @@
         <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -7504,16 +7508,16 @@
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -7521,16 +7525,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C20" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -7538,16 +7542,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -7555,16 +7559,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -7572,16 +7576,16 @@
         <v>25</v>
       </c>
       <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D23" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -7589,16 +7593,16 @@
         <v>26</v>
       </c>
       <c r="B24" s="2">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D24" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -7606,17 +7610,21 @@
         <v>27</v>
       </c>
       <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.6</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0.2261</v>
+      </c>
+      <c r="D25" s="16">
+        <v>0.2261</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M64" s="16"/>
+      <c r="N64" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fetching Cost and GHG emissions from feedstock
This change now makes it so that average cost and green house gas emissions of specific energy carriers are fetched from the individual feedstock tabs instead of the overview and cleans up the overview tab accordingly.
IMPORTANT: This does not make cost and greenhouse gas emissions time-bound and does not introduce a differentiation between buying and selling price!
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/FEEDSTOCKS.xlsx
+++ b/cea/databases/CH/components/FEEDSTOCKS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A982472-3F41-B441-95FC-85BAC176F9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55508D0-6115-4D27-BA0B-2DAC9297D06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="500" windowWidth="46580" windowHeight="27340" tabRatio="993" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="993" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRID" sheetId="28" r:id="rId1"/>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="154">
   <si>
     <t>reference</t>
   </si>
@@ -894,12 +894,6 @@
     <t>mean_qual</t>
   </si>
   <si>
-    <t>unit_cost_USD.kWh</t>
-  </si>
-  <si>
-    <t>unit_ghg_kgCO2.kWh</t>
-  </si>
-  <si>
     <t>Hot air</t>
   </si>
   <si>
@@ -1133,13 +1127,34 @@
     <t>Infrared light</t>
   </si>
   <si>
-    <t>This should be linked to GRID Tab</t>
-  </si>
-  <si>
-    <t>to be deleted</t>
-  </si>
-  <si>
-    <t>Shall we update the SOLAR Tab and change everything to zero?</t>
+    <t>cost_and_ghg_tab</t>
+  </si>
+  <si>
+    <t>GRID</t>
+  </si>
+  <si>
+    <t>WOOD</t>
+  </si>
+  <si>
+    <t>WETBIOMASS</t>
+  </si>
+  <si>
+    <t>DRYBIOMASS</t>
+  </si>
+  <si>
+    <t>COAL</t>
+  </si>
+  <si>
+    <t>OIL</t>
+  </si>
+  <si>
+    <t>NATURALGAS</t>
+  </si>
+  <si>
+    <t>BIOGAS</t>
+  </si>
+  <si>
+    <t>HYDROGEN</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1162,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1221,7 +1236,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1243,12 +1258,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,9 +1302,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1306,14 +1313,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1334,13 +1341,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1355,7 +1362,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1367,22 +1374,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -1826,16 +1822,16 @@
       <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1852,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1868,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1892,7 +1888,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1912,7 +1908,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1952,7 +1948,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1972,7 +1968,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1992,7 +1988,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2012,7 +2008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2032,7 +2028,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -2052,7 +2048,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2072,7 +2068,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -2092,7 +2088,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -2112,7 +2108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2132,7 +2128,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2152,7 +2148,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -2172,7 +2168,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -2192,7 +2188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -2212,7 +2208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -2232,7 +2228,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -2252,7 +2248,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2272,7 +2268,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -2292,7 +2288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -2312,7 +2308,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -2346,20 +2342,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2376,7 +2372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2393,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -2410,7 +2406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2427,7 +2423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -2444,7 +2440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -2461,7 +2457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -2478,7 +2474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2495,7 +2491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2512,7 +2508,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2529,7 +2525,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -2546,7 +2542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2563,7 +2559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -2580,7 +2576,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -2597,7 +2593,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2614,7 +2610,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2631,7 +2627,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -2648,7 +2644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -2665,7 +2661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -2682,7 +2678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -2699,7 +2695,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -2716,7 +2712,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2733,7 +2729,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -2750,7 +2746,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -2767,7 +2763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -2792,19 +2788,17 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468519ED-3798-6A47-8D33-1999B16E1C77}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="9" width="10.83203125" style="21"/>
-    <col min="10" max="10" width="102.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" customWidth="1"/>
+    <col min="9" max="9" width="102.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="19" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>61</v>
       </c>
@@ -2826,803 +2820,717 @@
       <c r="G1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="B2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="G2" s="10">
         <v>100</v>
       </c>
-      <c r="H2" s="23">
-        <v>0</v>
-      </c>
-      <c r="I2" s="23">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="G3" s="10">
         <v>35</v>
       </c>
-      <c r="H3" s="24">
-        <v>0</v>
-      </c>
-      <c r="I3" s="24">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="G4" s="10">
         <v>25</v>
       </c>
-      <c r="H4" s="24">
-        <v>0</v>
-      </c>
-      <c r="I4" s="24">
-        <v>0</v>
-      </c>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="G5" s="12">
         <v>10</v>
       </c>
-      <c r="H5" s="24">
-        <v>0</v>
-      </c>
-      <c r="I5" s="24">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G6" s="12">
         <v>0</v>
       </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-      <c r="I6" s="24">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G7" s="10">
         <v>100</v>
       </c>
-      <c r="H7" s="23">
-        <v>0</v>
-      </c>
-      <c r="I7" s="23">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F8" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G8" s="10">
         <v>60</v>
       </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-      <c r="I8" s="24">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G9" s="10">
         <v>30</v>
       </c>
-      <c r="H9" s="24">
-        <v>0</v>
-      </c>
-      <c r="I9" s="24">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F10" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G10" s="10">
         <v>20</v>
       </c>
-      <c r="H10" s="24">
-        <v>0</v>
-      </c>
-      <c r="I10" s="24">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F11" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G11" s="12">
         <v>10</v>
       </c>
-      <c r="H11" s="24">
-        <v>0</v>
-      </c>
-      <c r="I11" s="24">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="F12" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G12" s="10">
         <v>0</v>
       </c>
-      <c r="H12" s="24">
-        <v>0</v>
-      </c>
-      <c r="I12" s="24">
-        <v>0</v>
-      </c>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="82" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="E13" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="F13" s="16" t="s">
         <v>101</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="G13" s="17">
         <v>230</v>
       </c>
-      <c r="H13" s="25">
-        <v>0.21</v>
-      </c>
-      <c r="I13" s="25">
-        <v>0.40570000000000001</v>
-      </c>
-      <c r="J13" s="15" t="s">
+      <c r="H13" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="K13" s="21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="C14" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="G14" s="10">
         <v>22000</v>
       </c>
-      <c r="H14" s="23">
-        <v>0.18</v>
-      </c>
-      <c r="I14" s="25">
-        <v>0.40570000000000001</v>
-      </c>
-      <c r="J14" s="15" t="s">
+      <c r="H14" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="C15" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="F15" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="G15" s="10">
         <v>66000</v>
       </c>
-      <c r="H15" s="24">
-        <v>0.18</v>
-      </c>
-      <c r="I15" s="25">
-        <v>0.40570000000000001</v>
-      </c>
-      <c r="J15" s="15" t="s">
+      <c r="H15" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="C16" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="E16" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="F16" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G16" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="11" t="s">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="I16" s="24">
-        <v>2.7E-2</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="B17" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="C17" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="7" t="s">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="B18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="F18" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="I17" s="24">
-        <v>2.8799999999999999E-2</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="G18" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C19" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="F19" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="I18" s="24">
-        <v>2.8799999999999999E-2</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="G19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="E20" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="I19" s="24">
-        <v>0.41760000000000003</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="F20" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="7" t="s">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="B21" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="24">
-        <v>0.08</v>
-      </c>
-      <c r="I20" s="24">
-        <v>0.3024</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="F21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="B22" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H21" s="24">
-        <v>0.09</v>
-      </c>
-      <c r="I21" s="20">
-        <v>0.24060000000000001</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="F22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="7" t="s">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="B23" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="F23" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="24">
-        <v>0.17</v>
-      </c>
-      <c r="I22" s="24">
-        <v>0.12959999999999999</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="G23" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="14" t="s">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="B24" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="25">
-        <v>0.2261</v>
-      </c>
-      <c r="I23" s="25">
-        <v>1.9300000000000001E-2</v>
-      </c>
-      <c r="J23" s="4" t="s">
+      <c r="E24" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="C25" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="D25" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H24" s="24">
-        <v>0</v>
-      </c>
-      <c r="I24" s="24">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15" t="s">
+      <c r="F25" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="K24" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="G25" s="12">
         <v>200</v>
       </c>
-      <c r="H25" s="24">
-        <v>0</v>
-      </c>
-      <c r="I25" s="24">
-        <v>0</v>
-      </c>
-      <c r="J25" s="15" t="s">
+      <c r="H25" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="G26" s="12">
         <v>1500</v>
       </c>
-      <c r="H26" s="24">
-        <v>0</v>
-      </c>
-      <c r="I26" s="24">
-        <v>0</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H27" s="21" t="s">
-        <v>147</v>
+      <c r="H26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3638,16 +3546,16 @@
       <selection activeCell="E2" sqref="E2:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3664,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3684,7 +3592,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3704,7 +3612,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -3724,7 +3632,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -3744,7 +3652,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -3764,7 +3672,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -3784,7 +3692,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3804,7 +3712,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -3824,7 +3732,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -3844,7 +3752,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -3864,7 +3772,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -3884,7 +3792,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -3904,7 +3812,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -3924,7 +3832,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -3944,7 +3852,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -3964,7 +3872,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -3984,7 +3892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -4004,7 +3912,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -4024,7 +3932,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -4044,7 +3952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -4064,7 +3972,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -4084,7 +3992,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -4104,7 +4012,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -4124,7 +4032,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -4161,16 +4069,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4187,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -4207,7 +4115,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -4227,7 +4135,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -4247,7 +4155,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -4267,7 +4175,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -4287,7 +4195,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -4307,7 +4215,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4327,7 +4235,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4347,7 +4255,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -4367,7 +4275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -4387,7 +4295,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -4407,7 +4315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -4427,7 +4335,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -4447,7 +4355,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -4467,7 +4375,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -4487,7 +4395,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -4507,7 +4415,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -4527,7 +4435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -4547,7 +4455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -4567,7 +4475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -4587,7 +4495,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -4607,7 +4515,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -4627,7 +4535,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -4647,7 +4555,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -4681,16 +4589,16 @@
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4707,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -4727,7 +4635,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -4747,7 +4655,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -4767,7 +4675,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -4787,7 +4695,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -4807,7 +4715,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -4827,7 +4735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4847,7 +4755,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4867,7 +4775,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -4887,7 +4795,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -4907,7 +4815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -4927,7 +4835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -4947,7 +4855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -4967,7 +4875,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -4987,7 +4895,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -5007,7 +4915,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -5027,7 +4935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -5047,7 +4955,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -5067,7 +4975,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -5087,7 +4995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -5107,7 +5015,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -5127,7 +5035,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -5147,7 +5055,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -5167,7 +5075,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -5201,16 +5109,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -5227,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -5247,7 +5155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -5267,7 +5175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -5287,7 +5195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -5307,7 +5215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -5327,7 +5235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -5347,7 +5255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5367,7 +5275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5387,7 +5295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5407,7 +5315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -5427,7 +5335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -5447,7 +5355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -5467,7 +5375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -5487,7 +5395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -5507,7 +5415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -5527,7 +5435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -5547,7 +5455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -5567,7 +5475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -5587,7 +5495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -5607,7 +5515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -5627,7 +5535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -5647,7 +5555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -5667,7 +5575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -5687,7 +5595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -5721,16 +5629,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -5747,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -5767,7 +5675,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -5787,7 +5695,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -5807,7 +5715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -5827,7 +5735,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -5847,7 +5755,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -5867,7 +5775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5887,7 +5795,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5907,7 +5815,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5927,7 +5835,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -5947,7 +5855,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -5967,7 +5875,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -5987,7 +5895,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -6007,7 +5915,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -6027,7 +5935,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -6047,7 +5955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -6067,7 +5975,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -6087,7 +5995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -6107,7 +6015,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -6127,7 +6035,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -6147,7 +6055,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -6167,7 +6075,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -6187,7 +6095,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -6207,7 +6115,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -6241,16 +6149,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6267,7 +6175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -6285,7 +6193,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -6303,7 +6211,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -6321,7 +6229,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -6339,7 +6247,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -6357,7 +6265,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -6375,7 +6283,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6393,7 +6301,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6411,7 +6319,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6429,7 +6337,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -6447,7 +6355,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -6465,7 +6373,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -6483,7 +6391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -6501,7 +6409,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -6519,7 +6427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -6537,7 +6445,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -6555,7 +6463,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -6573,7 +6481,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -6591,7 +6499,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -6609,7 +6517,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -6627,7 +6535,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -6645,7 +6553,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -6663,7 +6571,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -6681,7 +6589,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -6716,16 +6624,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6742,7 +6650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -6760,7 +6668,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -6778,7 +6686,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -6796,7 +6704,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -6814,7 +6722,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -6832,7 +6740,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -6850,7 +6758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6868,7 +6776,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6886,7 +6794,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6904,7 +6812,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -6922,7 +6830,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -6940,7 +6848,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -6958,7 +6866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -6976,7 +6884,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -6994,7 +6902,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -7012,7 +6920,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -7030,7 +6938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -7048,7 +6956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -7066,7 +6974,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -7084,7 +6992,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -7102,7 +7010,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -7120,7 +7028,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -7138,7 +7046,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -7156,7 +7064,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -7191,13 +7099,13 @@
       <selection activeCell="P73" sqref="I48:P73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -7214,7 +7122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -7228,10 +7136,10 @@
         <v>0.2261</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -7245,10 +7153,10 @@
         <v>0.2261</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -7262,10 +7170,10 @@
         <v>0.2261</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -7279,10 +7187,10 @@
         <v>0.2261</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -7296,10 +7204,10 @@
         <v>0.2261</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -7313,10 +7221,10 @@
         <v>0.2261</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -7330,10 +7238,10 @@
         <v>0.2261</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -7347,10 +7255,10 @@
         <v>0.2261</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -7364,10 +7272,10 @@
         <v>0.2261</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -7381,10 +7289,10 @@
         <v>0.2261</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -7398,10 +7306,10 @@
         <v>0.2261</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -7415,10 +7323,10 @@
         <v>0.2261</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -7432,10 +7340,10 @@
         <v>0.2261</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -7449,10 +7357,10 @@
         <v>0.2261</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -7466,10 +7374,10 @@
         <v>0.2261</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -7483,10 +7391,10 @@
         <v>0.2261</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -7500,10 +7408,10 @@
         <v>0.2261</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -7517,10 +7425,10 @@
         <v>0.2261</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -7534,10 +7442,10 @@
         <v>0.2261</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -7551,10 +7459,10 @@
         <v>0.2261</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -7568,10 +7476,10 @@
         <v>0.2261</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -7585,10 +7493,10 @@
         <v>0.2261</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -7602,10 +7510,10 @@
         <v>0.2261</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -7619,10 +7527,10 @@
         <v>0.2261</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="64" spans="13:14" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
     </row>

</xml_diff>